<commit_message>
Aggiunti commenti su Kruskal e confronto algoritmi
</commit_message>
<xml_diff>
--- a/Relazione/grafici.xlsx
+++ b/Relazione/grafici.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Algoritmi-Avanzati\Relazione\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88C9DF9-7836-4950-98F5-D76B542207CB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93204258-3971-4156-AB67-385F3A192EC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="11385" activeTab="3" xr2:uid="{DDB9F065-D234-BE46-AFC7-AD61ACD45C34}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>Nodi</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>Kruskal</t>
+  </si>
+  <si>
+    <t>PrimRispetto a kruskal UF</t>
+  </si>
+  <si>
+    <t>Kruskal rispetto a Kruskal Uf</t>
   </si>
 </sst>
 </file>
@@ -161,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -177,6 +183,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -4884,6 +4891,1112 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800"/>
+              <a:t>Prim vs Kruskal con Union-Find</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Numero di grafi elaborati da Prim</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Medie!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Medie!$F$2:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9375</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.875</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.90625</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12.061538461538461</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.553571428571427</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14.860544217687075</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000013-A495-4946-88E5-BB755FF2D4DD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="-25"/>
+        <c:axId val="916616703"/>
+        <c:axId val="1002532287"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="916616703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="1100"/>
+                  <a:t>Numero nodi</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1002532287"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1002532287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="1100"/>
+                  <a:t>Numero grafi</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="1100" baseline="0"/>
+                  <a:t> elaborati</a:t>
+                </a:r>
+                <a:endParaRPr lang="it-IT" sz="1100"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="916616703"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="360"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="106"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="6"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800"/>
+              <a:t>Kruskal Naive vs Kruskal con Union-Find</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Numero di grafi elaborati da Kruskal Naive</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Medie!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Medie!$G$2:$G$18</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.8125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>106.9375</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>230.63333333333333</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>652.4375</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1606.6875</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5056.7538461538461</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12386.107142857143</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12322.299319727892</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3AAC-4ABC-B943-6FE2D3853351}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="-25"/>
+        <c:axId val="916616703"/>
+        <c:axId val="1002532287"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="916616703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="1200"/>
+                  <a:t>Numero nodi</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1002532287"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1002532287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="1200"/>
+                  <a:t>Numero grafi</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="1200" baseline="0"/>
+                  <a:t> elaborati</a:t>
+                </a:r>
+                <a:endParaRPr lang="it-IT" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="916616703"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="360"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
@@ -5072,6 +6185,52 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
+  <a:schemeClr val="accent4"/>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="269">
   <cs:axisTitle>
@@ -7652,6 +8811,1012 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -7836,16 +10001,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>433387</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>128587</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>204787</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>585787</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7865,6 +10030,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>119062</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>80960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>32662</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>160610</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA010FC1-72A7-4123-8A3D-89FE499486D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2447924</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>79650</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Grafico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3400050-9CDA-4597-82A3-686FB93A4EF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8965,7 +11204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB48406B-403F-7948-A64C-7034AE57827E}">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="L45" sqref="L45:L61"/>
     </sheetView>
   </sheetViews>
@@ -10577,15 +12816,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172D2086-63C8-4A75-9B95-F8D3E0C0BB2D}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="20.375" customWidth="1"/>
+    <col min="7" max="7" width="32.125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -10598,8 +12841,14 @@
       <c r="D1" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>10</v>
       </c>
@@ -10615,8 +12864,16 @@
         <f>AVERAGEIF(Kruskal!A2:A69,Kruskal!J31,Kruskal!B2:B69)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="9">
+        <f>IF(C2=0, B2/1,B2/C2)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="9">
+        <f>IF(C2=0, D2/1,D2/C2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>20</v>
       </c>
@@ -10632,8 +12889,16 @@
         <f>AVERAGEIF(Kruskal!A3:A70,Kruskal!J32,Kruskal!B3:B70)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="9">
+        <f t="shared" ref="F3:F19" si="0">IF(C3=0, B3/1,B3/C3)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" ref="G3:G18" si="1">IF(C3=0, D3/1,D3/C3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>40</v>
       </c>
@@ -10649,8 +12914,16 @@
         <f>AVERAGEIF(Kruskal!A4:A71,Kruskal!J33,Kruskal!B4:B71)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>80</v>
       </c>
@@ -10666,8 +12939,16 @@
         <f>AVERAGEIF(Kruskal!A5:A72,Kruskal!J34,Kruskal!B5:B72)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>100</v>
       </c>
@@ -10683,8 +12964,16 @@
         <f>AVERAGEIF(Kruskal!A6:A73,Kruskal!J35,Kruskal!B6:B73)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>200</v>
       </c>
@@ -10700,8 +12989,16 @@
         <f>AVERAGEIF(Kruskal!A7:A74,Kruskal!J36,Kruskal!B7:B74)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>400</v>
       </c>
@@ -10717,8 +13014,16 @@
         <f>AVERAGEIF(Kruskal!A8:A75,Kruskal!J37,Kruskal!B8:B75)</f>
         <v>7.75</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="9">
+        <f t="shared" si="1"/>
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>800</v>
       </c>
@@ -10734,8 +13039,16 @@
         <f>AVERAGEIF(Kruskal!A9:A76,Kruskal!J38,Kruskal!B9:B76)</f>
         <v>27.25</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="9">
+        <f t="shared" si="1"/>
+        <v>6.8125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>1000</v>
       </c>
@@ -10751,8 +13064,16 @@
         <f>AVERAGEIF(Kruskal!A10:A77,Kruskal!J39,Kruskal!B10:B77)</f>
         <v>31.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10" s="9">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
+      <c r="G10" s="9">
+        <f t="shared" si="1"/>
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>2000</v>
       </c>
@@ -10768,8 +13089,16 @@
         <f>AVERAGEIF(Kruskal!A11:A78,Kruskal!J40,Kruskal!B11:B78)</f>
         <v>109</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F11" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="9">
+        <f t="shared" si="1"/>
+        <v>27.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>4000</v>
       </c>
@@ -10785,8 +13114,16 @@
         <f>AVERAGEIF(Kruskal!A12:A79,Kruskal!J41,Kruskal!B12:B79)</f>
         <v>427.75</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F12" s="9">
+        <f t="shared" si="0"/>
+        <v>1.9375</v>
+      </c>
+      <c r="G12" s="9">
+        <f t="shared" si="1"/>
+        <v>106.9375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>8000</v>
       </c>
@@ -10802,8 +13139,16 @@
         <f>AVERAGEIF(Kruskal!A13:A80,Kruskal!J42,Kruskal!B13:B80)</f>
         <v>1729.75</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F13" s="9">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+      <c r="G13" s="9">
+        <f t="shared" si="1"/>
+        <v>230.63333333333333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>10000</v>
       </c>
@@ -10819,8 +13164,16 @@
         <f>AVERAGEIF(Kruskal!A14:A81,Kruskal!J43,Kruskal!B14:B81)</f>
         <v>2609.75</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F14" s="9">
+        <f t="shared" si="0"/>
+        <v>4.875</v>
+      </c>
+      <c r="G14" s="9">
+        <f t="shared" si="1"/>
+        <v>652.4375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>20000</v>
       </c>
@@ -10836,8 +13189,16 @@
         <f>AVERAGEIF(Kruskal!A15:A82,Kruskal!J44,Kruskal!B15:B82)</f>
         <v>12853.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F15" s="9">
+        <f t="shared" si="0"/>
+        <v>7.90625</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" si="1"/>
+        <v>1606.6875</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>40000</v>
       </c>
@@ -10853,8 +13214,16 @@
         <f>AVERAGEIF(Kruskal!A16:A83,Kruskal!J45,Kruskal!B16:B83)</f>
         <v>82172.25</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" s="9">
+        <f>IF(C16=0, B16/1,B16/C16)</f>
+        <v>12.061538461538461</v>
+      </c>
+      <c r="G16" s="9">
+        <f t="shared" si="1"/>
+        <v>5056.7538461538461</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>80000</v>
       </c>
@@ -10870,8 +13239,16 @@
         <f>AVERAGEIF(Kruskal!A17:A84,Kruskal!J46,Kruskal!B17:B84)</f>
         <v>520216.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17" s="9">
+        <f t="shared" si="0"/>
+        <v>16.553571428571427</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" si="1"/>
+        <v>12386.107142857143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>100000</v>
       </c>
@@ -10887,10 +13264,18 @@
         <f>AVERAGEIF(Kruskal!A18:A85,Kruskal!J47,Kruskal!B18:B85)</f>
         <v>905689</v>
       </c>
+      <c r="F18" s="9">
+        <f t="shared" si="0"/>
+        <v>14.860544217687075</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="1"/>
+        <v>12322.299319727892</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>